<commit_message>
Update project03 - 요구사항 정의서 - 현태.xlsx
</commit_message>
<xml_diff>
--- a/project03 - 요구사항 정의서 - 현태.xlsx
+++ b/project03 - 요구사항 정의서 - 현태.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="144">
   <si>
     <t>로그인 및 계정관련</t>
   </si>
@@ -216,120 +216,14 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>로그인</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원가입</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>마이페이지</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>리워드 펀딩 프로젝트 등록</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>베스트 프로젝트 확인</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>카테고리별 프로젝트 확인</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>다가올 펀딩 미리 보기</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로젝트 신고</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>지나간 프로젝트 확인</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>관심 프로젝트 등록</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>공지사항</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>Q&amp;A</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>펀딩</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>하는</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>방법</t>
-    </r>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>실시간 상담</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>채팅 상담</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>회원관리</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>등록 신청 프로젝트 검토 및 승인</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>카테고리 관리</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>프로젝트 관리</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
@@ -339,30 +233,6 @@
   </si>
   <si>
     <t>커뮤니티 관리</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>펀딩하는 방법</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>결제 관리</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>실시간 채팅 관리</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>메인 화면 관리</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>통계 관리</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>예치금 관리</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
@@ -530,27 +400,7 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>프로젝트 제작 회원 (메이커)</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로젝트 투자 회원 (서포터)</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>투자 펀딩 프로젝트 등록</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>관리자</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>메인 화면 (진입 화면)</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>메인 화면 (진입 화면)</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
@@ -605,10 +455,6 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>프로젝트 관련 자유 게시판 및 토론 게시판</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>최근 이슈 및 회사 운영 관련 공지사항</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
@@ -622,10 +468,6 @@
   </si>
   <si>
     <t>관심 프로젝트로 등록 후 마이페이지에서 모아보기 및 펀딩 할 수 있도록 설정</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>관리자와의 실시간 채팅을 통한 상담 (로그인 필수)</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
@@ -1001,6 +843,250 @@
 - 프로젝트 이름, 펀딩 받을 목표금액, 상품 가격, 프로젝트 진행 기간, 프로젝트 고유 주소, 프로젝트 대표 이미지, 프로젝트 키워드, 프로젝트 세부 동영상, 프로젝트 세부 이미지, 프로젝트 세부 내용, 리워드 세부내용, 환불 정책, 문의 가능 번호, 사업자 등록 번호 </t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
+  <si>
+    <t>관리자와의 실시간 채팅을 통한 상담 (로그인 필수)
+- 모든 페이지 오른쪽 하단 플로팅 배너</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인 화면 및 실시간 채팅</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>계정 관련</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>메이커 회원 프로젝트 등록</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>서포터 회원 프로젝트 펀딩</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시판 관련</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인 화면</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원 관리</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 관리</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>커뮤니티 관리</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>결제 관리</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>통계</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>실시간 채팅 관리
+메인화면 관리</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인 (1)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원가입 (1)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>마이페이지 (5)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>예치금 관리 (-)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인 화면 (진입 화면) (1)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>투자 펀딩 프로젝트 등록 (3)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>리워드 펀딩 프로젝트 등록 (3)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인 화면 (진입 화면) (1+1)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>베스트 프로젝트 확인 (1)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>지나간 프로젝트 확인 (1)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>다가올 펀딩 미리 보기 (1)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 신고 (-)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>관심 프로젝트 등록 (-)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 관련 자유 게시판 및 토론 게시판 (1)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>공지사항 (1)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q&amp;A (1)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>펀딩</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>하는</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>방법</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (1)</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>채팅 상담 (1)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 제작 회원 (메이커) (1)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로젝트 투자 회원 (서포터) (1)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>등록 신청 프로젝트 검토 및 승인 (1)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>카테고리 관리 (1)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>통계 관리 (1)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>펀딩하는 방법 (1)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>결제 관리 (1)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>실시간 채팅 관리 (1)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인 화면 관리 (1)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>카테고리별 프로젝트 확인 (1+1+1)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -1120,7 +1206,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -1596,11 +1682,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1758,94 +1855,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1878,9 +1891,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1899,6 +1909,42 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1916,6 +1962,82 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2134,19 +2256,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11.85546875" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="135.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="24.140625" customWidth="1"/>
     <col min="10" max="10" width="18.140625" customWidth="1"/>
     <col min="11" max="11" width="19" customWidth="1"/>
@@ -2193,22 +2315,22 @@
     </row>
     <row r="2" spans="1:33" ht="19.5" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="55"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="100"/>
+      <c r="M2" s="100"/>
+      <c r="N2" s="100"/>
+      <c r="O2" s="101"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
@@ -2230,20 +2352,20 @@
     </row>
     <row r="3" spans="1:33" ht="19.5" customHeight="1" thickBot="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="56"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="58"/>
+      <c r="B3" s="102"/>
+      <c r="C3" s="103"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="103"/>
+      <c r="H3" s="103"/>
+      <c r="I3" s="103"/>
+      <c r="J3" s="103"/>
+      <c r="K3" s="103"/>
+      <c r="L3" s="103"/>
+      <c r="M3" s="103"/>
+      <c r="N3" s="103"/>
+      <c r="O3" s="104"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
@@ -2369,13 +2491,13 @@
       <c r="AG6" s="1"/>
     </row>
     <row r="7" spans="1:33" ht="27.75" customHeight="1">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="75" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="22" t="s">
@@ -2384,29 +2506,29 @@
       <c r="E7" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="59" t="s">
+      <c r="F7" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="59" t="s">
+      <c r="G7" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="59"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="59"/>
-      <c r="K7" s="59"/>
-      <c r="L7" s="59" t="s">
+      <c r="H7" s="75"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="59" t="s">
+      <c r="M7" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="N7" s="60" t="s">
+      <c r="N7" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="O7" s="62" t="s">
+      <c r="O7" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="P7" s="62" t="s">
+      <c r="P7" s="89" t="s">
         <v>17</v>
       </c>
       <c r="Q7" s="1"/>
@@ -2428,12 +2550,12 @@
       <c r="AG7" s="1"/>
     </row>
     <row r="8" spans="1:33" ht="27.75" customHeight="1">
-      <c r="A8" s="59"/>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
+      <c r="A8" s="75"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
-      <c r="F8" s="59"/>
+      <c r="F8" s="75"/>
       <c r="G8" s="23">
         <v>43854</v>
       </c>
@@ -2449,11 +2571,11 @@
       <c r="K8" s="23">
         <v>43861</v>
       </c>
-      <c r="L8" s="59"/>
-      <c r="M8" s="59"/>
-      <c r="N8" s="61"/>
-      <c r="O8" s="63"/>
-      <c r="P8" s="63"/>
+      <c r="L8" s="75"/>
+      <c r="M8" s="75"/>
+      <c r="N8" s="106"/>
+      <c r="O8" s="90"/>
+      <c r="P8" s="90"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
@@ -2473,15 +2595,15 @@
       <c r="AG8" s="1"/>
     </row>
     <row r="9" spans="1:33" ht="27.75" customHeight="1">
-      <c r="A9" s="100" t="s">
+      <c r="A9" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="71" t="s">
-        <v>92</v>
-      </c>
-      <c r="C9" s="72"/>
-      <c r="D9" s="89" t="s">
-        <v>107</v>
+      <c r="B9" s="97" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="98"/>
+      <c r="D9" s="61" t="s">
+        <v>79</v>
       </c>
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
@@ -2520,15 +2642,15 @@
       <c r="AG9" s="1"/>
     </row>
     <row r="10" spans="1:33" ht="27.75" customHeight="1">
-      <c r="A10" s="101"/>
-      <c r="B10" s="73" t="s">
+      <c r="A10" s="84"/>
+      <c r="B10" s="78" t="s">
         <v>57</v>
       </c>
       <c r="C10" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="97" t="s">
-        <v>94</v>
+        <v>111</v>
+      </c>
+      <c r="D10" s="68" t="s">
+        <v>67</v>
       </c>
       <c r="E10" s="21"/>
       <c r="F10" s="21"/>
@@ -2567,13 +2689,13 @@
       <c r="AG10" s="1"/>
     </row>
     <row r="11" spans="1:33" ht="27.75" customHeight="1">
-      <c r="A11" s="101"/>
-      <c r="B11" s="70"/>
+      <c r="A11" s="84"/>
+      <c r="B11" s="79"/>
       <c r="C11" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="90" t="s">
-        <v>103</v>
+        <v>112</v>
+      </c>
+      <c r="D11" s="62" t="s">
+        <v>76</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -2612,13 +2734,13 @@
       <c r="AG11" s="1"/>
     </row>
     <row r="12" spans="1:33" ht="60">
-      <c r="A12" s="101"/>
-      <c r="B12" s="70"/>
+      <c r="A12" s="84"/>
+      <c r="B12" s="79"/>
       <c r="C12" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="90" t="s">
-        <v>95</v>
+        <v>113</v>
+      </c>
+      <c r="D12" s="62" t="s">
+        <v>68</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -2657,13 +2779,13 @@
       <c r="AG12" s="1"/>
     </row>
     <row r="13" spans="1:33" ht="27.75" customHeight="1">
-      <c r="A13" s="101"/>
-      <c r="B13" s="74"/>
+      <c r="A13" s="84"/>
+      <c r="B13" s="80"/>
       <c r="C13" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="D13" s="90" t="s">
-        <v>96</v>
+        <v>114</v>
+      </c>
+      <c r="D13" s="62" t="s">
+        <v>69</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -2696,15 +2818,15 @@
       <c r="AG13" s="1"/>
     </row>
     <row r="14" spans="1:33" ht="36">
-      <c r="A14" s="101"/>
-      <c r="B14" s="67" t="s">
-        <v>85</v>
+      <c r="A14" s="84"/>
+      <c r="B14" s="94" t="s">
+        <v>63</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="D14" s="90" t="s">
-        <v>97</v>
+        <v>116</v>
+      </c>
+      <c r="D14" s="62" t="s">
+        <v>70</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -2743,13 +2865,13 @@
       <c r="AG14" s="1"/>
     </row>
     <row r="15" spans="1:33" ht="36">
-      <c r="A15" s="101"/>
-      <c r="B15" s="68"/>
+      <c r="A15" s="84"/>
+      <c r="B15" s="95"/>
       <c r="C15" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="90" t="s">
-        <v>124</v>
+        <v>117</v>
+      </c>
+      <c r="D15" s="62" t="s">
+        <v>95</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -2788,15 +2910,15 @@
       <c r="AG15" s="1"/>
     </row>
     <row r="16" spans="1:33" ht="36">
-      <c r="A16" s="101"/>
-      <c r="B16" s="67" t="s">
-        <v>86</v>
+      <c r="A16" s="84"/>
+      <c r="B16" s="94" t="s">
+        <v>64</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="90" t="s">
-        <v>98</v>
+        <v>138</v>
+      </c>
+      <c r="D16" s="62" t="s">
+        <v>71</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -2835,13 +2957,13 @@
       <c r="AG16" s="1"/>
     </row>
     <row r="17" spans="1:33" ht="36">
-      <c r="A17" s="101"/>
-      <c r="B17" s="69"/>
+      <c r="A17" s="84"/>
+      <c r="B17" s="96"/>
       <c r="C17" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="90" t="s">
-        <v>99</v>
+        <v>119</v>
+      </c>
+      <c r="D17" s="62" t="s">
+        <v>72</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -2880,13 +3002,13 @@
       <c r="AG17" s="1"/>
     </row>
     <row r="18" spans="1:33" ht="27.75" customHeight="1">
-      <c r="A18" s="101"/>
-      <c r="B18" s="69"/>
+      <c r="A18" s="84"/>
+      <c r="B18" s="96"/>
       <c r="C18" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="90" t="s">
-        <v>100</v>
+        <v>120</v>
+      </c>
+      <c r="D18" s="62" t="s">
+        <v>73</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -2925,13 +3047,13 @@
       <c r="AG18" s="1"/>
     </row>
     <row r="19" spans="1:33" ht="27.75" customHeight="1">
-      <c r="A19" s="101"/>
-      <c r="B19" s="69"/>
+      <c r="A19" s="84"/>
+      <c r="B19" s="96"/>
       <c r="C19" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="90" t="s">
-        <v>102</v>
+        <v>121</v>
+      </c>
+      <c r="D19" s="62" t="s">
+        <v>75</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -2970,13 +3092,13 @@
       <c r="AG19" s="1"/>
     </row>
     <row r="20" spans="1:33" ht="27.75" customHeight="1">
-      <c r="A20" s="101"/>
-      <c r="B20" s="69"/>
+      <c r="A20" s="84"/>
+      <c r="B20" s="96"/>
       <c r="C20" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="91" t="s">
-        <v>101</v>
+        <v>122</v>
+      </c>
+      <c r="D20" s="63" t="s">
+        <v>74</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -3015,13 +3137,13 @@
       <c r="AG20" s="1"/>
     </row>
     <row r="21" spans="1:33" ht="27.75" customHeight="1">
-      <c r="A21" s="101"/>
-      <c r="B21" s="68"/>
+      <c r="A21" s="84"/>
+      <c r="B21" s="95"/>
       <c r="C21" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" s="92" t="s">
-        <v>108</v>
+        <v>123</v>
+      </c>
+      <c r="D21" s="64" t="s">
+        <v>80</v>
       </c>
       <c r="E21" s="51"/>
       <c r="F21" s="16"/>
@@ -3060,15 +3182,15 @@
       <c r="AG21" s="1"/>
     </row>
     <row r="22" spans="1:33" ht="27.75" customHeight="1">
-      <c r="A22" s="101"/>
-      <c r="B22" s="64" t="s">
-        <v>87</v>
+      <c r="A22" s="84"/>
+      <c r="B22" s="91" t="s">
+        <v>65</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="D22" s="90" t="s">
-        <v>110</v>
+        <v>124</v>
+      </c>
+      <c r="D22" s="62" t="s">
+        <v>81</v>
       </c>
       <c r="E22" s="11"/>
       <c r="F22" s="12"/>
@@ -3103,13 +3225,13 @@
       <c r="AG22" s="1"/>
     </row>
     <row r="23" spans="1:33" ht="27.75" customHeight="1">
-      <c r="A23" s="101"/>
-      <c r="B23" s="65"/>
+      <c r="A23" s="84"/>
+      <c r="B23" s="92"/>
       <c r="C23" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="90" t="s">
-        <v>105</v>
+        <v>125</v>
+      </c>
+      <c r="D23" s="62" t="s">
+        <v>77</v>
       </c>
       <c r="E23" s="11"/>
       <c r="F23" s="15"/>
@@ -3148,13 +3270,13 @@
       <c r="AG23" s="1"/>
     </row>
     <row r="24" spans="1:33" ht="27.75" customHeight="1">
-      <c r="A24" s="101"/>
-      <c r="B24" s="65"/>
+      <c r="A24" s="84"/>
+      <c r="B24" s="92"/>
       <c r="C24" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="D24" s="94" t="s">
-        <v>111</v>
+        <v>126</v>
+      </c>
+      <c r="D24" s="65" t="s">
+        <v>82</v>
       </c>
       <c r="E24" s="11"/>
       <c r="F24" s="15"/>
@@ -3193,13 +3315,13 @@
       <c r="AG24" s="1"/>
     </row>
     <row r="25" spans="1:33" ht="27.75" customHeight="1">
-      <c r="A25" s="101"/>
-      <c r="B25" s="66"/>
+      <c r="A25" s="84"/>
+      <c r="B25" s="93"/>
       <c r="C25" s="52" t="s">
-        <v>70</v>
-      </c>
-      <c r="D25" s="90" t="s">
-        <v>106</v>
+        <v>127</v>
+      </c>
+      <c r="D25" s="62" t="s">
+        <v>78</v>
       </c>
       <c r="E25" s="11"/>
       <c r="F25" s="15"/>
@@ -3237,16 +3359,16 @@
       <c r="AF25" s="1"/>
       <c r="AG25" s="1"/>
     </row>
-    <row r="26" spans="1:33" ht="27.75" customHeight="1" thickBot="1">
-      <c r="A26" s="102"/>
+    <row r="26" spans="1:33" ht="27" customHeight="1" thickBot="1">
+      <c r="A26" s="85"/>
       <c r="B26" s="32" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D26" s="93" t="s">
-        <v>109</v>
+        <v>128</v>
+      </c>
+      <c r="D26" s="107" t="s">
+        <v>96</v>
       </c>
       <c r="E26" s="33"/>
       <c r="F26" s="33"/>
@@ -3285,25 +3407,25 @@
       <c r="AG26" s="1"/>
     </row>
     <row r="27" spans="1:33" ht="27.75" customHeight="1" thickTop="1">
-      <c r="A27" s="103" t="s">
-        <v>91</v>
+      <c r="A27" s="86" t="s">
+        <v>66</v>
       </c>
       <c r="B27" s="81" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="C27" s="82"/>
-      <c r="D27" s="98" t="s">
-        <v>112</v>
-      </c>
-      <c r="E27" s="83"/>
-      <c r="F27" s="83"/>
-      <c r="G27" s="84"/>
-      <c r="H27" s="84"/>
-      <c r="I27" s="84"/>
-      <c r="J27" s="85"/>
-      <c r="K27" s="86"/>
-      <c r="L27" s="87"/>
-      <c r="M27" s="88"/>
+      <c r="D27" s="69" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" s="55"/>
+      <c r="F27" s="55"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="56"/>
+      <c r="J27" s="57"/>
+      <c r="K27" s="58"/>
+      <c r="L27" s="59"/>
+      <c r="M27" s="60"/>
       <c r="N27" s="8"/>
       <c r="O27" s="5"/>
       <c r="P27" s="5"/>
@@ -3326,15 +3448,15 @@
       <c r="AG27" s="1"/>
     </row>
     <row r="28" spans="1:33" ht="48">
-      <c r="A28" s="104"/>
-      <c r="B28" s="70" t="s">
-        <v>73</v>
+      <c r="A28" s="87"/>
+      <c r="B28" s="79" t="s">
+        <v>59</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="D28" s="97" t="s">
-        <v>123</v>
+        <v>129</v>
+      </c>
+      <c r="D28" s="68" t="s">
+        <v>94</v>
       </c>
       <c r="E28" s="31"/>
       <c r="F28" s="31"/>
@@ -3371,13 +3493,13 @@
       <c r="AG28" s="1"/>
     </row>
     <row r="29" spans="1:33" ht="48">
-      <c r="A29" s="104"/>
-      <c r="B29" s="70"/>
+      <c r="A29" s="87"/>
+      <c r="B29" s="79"/>
       <c r="C29" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D29" s="94" t="s">
-        <v>122</v>
+        <v>130</v>
+      </c>
+      <c r="D29" s="65" t="s">
+        <v>93</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
@@ -3414,15 +3536,15 @@
       <c r="AG29" s="1"/>
     </row>
     <row r="30" spans="1:33" ht="27.75" customHeight="1">
-      <c r="A30" s="104"/>
-      <c r="B30" s="79" t="s">
-        <v>76</v>
+      <c r="A30" s="87"/>
+      <c r="B30" s="76" t="s">
+        <v>60</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="D30" s="94" t="s">
-        <v>113</v>
+        <v>131</v>
+      </c>
+      <c r="D30" s="65" t="s">
+        <v>84</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
@@ -3459,13 +3581,13 @@
       <c r="AG30" s="1"/>
     </row>
     <row r="31" spans="1:33" ht="27.75" customHeight="1">
-      <c r="A31" s="104"/>
-      <c r="B31" s="80"/>
+      <c r="A31" s="87"/>
+      <c r="B31" s="77"/>
       <c r="C31" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D31" s="91" t="s">
-        <v>114</v>
+        <v>132</v>
+      </c>
+      <c r="D31" s="63" t="s">
+        <v>85</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
@@ -3502,15 +3624,15 @@
       <c r="AG31" s="1"/>
     </row>
     <row r="32" spans="1:33" ht="27.75" customHeight="1">
-      <c r="A32" s="104"/>
+      <c r="A32" s="87"/>
       <c r="B32" s="24" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="D32" s="95" t="s">
-        <v>115</v>
+        <v>133</v>
+      </c>
+      <c r="D32" s="66" t="s">
+        <v>86</v>
       </c>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
@@ -3545,15 +3667,15 @@
       <c r="AG32" s="1"/>
     </row>
     <row r="33" spans="1:33" ht="27.75" customHeight="1">
-      <c r="A33" s="104"/>
-      <c r="B33" s="73" t="s">
-        <v>78</v>
+      <c r="A33" s="87"/>
+      <c r="B33" s="78" t="s">
+        <v>62</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33" s="96" t="s">
-        <v>116</v>
+        <v>125</v>
+      </c>
+      <c r="D33" s="67" t="s">
+        <v>87</v>
       </c>
       <c r="E33" s="20"/>
       <c r="F33" s="20"/>
@@ -3586,13 +3708,13 @@
       <c r="AG33" s="1"/>
     </row>
     <row r="34" spans="1:33" ht="27.75" customHeight="1">
-      <c r="A34" s="104"/>
-      <c r="B34" s="70"/>
+      <c r="A34" s="87"/>
+      <c r="B34" s="79"/>
       <c r="C34" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="D34" s="96" t="s">
-        <v>117</v>
+        <v>126</v>
+      </c>
+      <c r="D34" s="67" t="s">
+        <v>88</v>
       </c>
       <c r="E34" s="20"/>
       <c r="F34" s="20"/>
@@ -3625,13 +3747,13 @@
       <c r="AG34" s="1"/>
     </row>
     <row r="35" spans="1:33" ht="27.75" customHeight="1">
-      <c r="A35" s="104"/>
-      <c r="B35" s="74"/>
+      <c r="A35" s="87"/>
+      <c r="B35" s="80"/>
       <c r="C35" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D35" s="96" t="s">
-        <v>118</v>
+        <v>134</v>
+      </c>
+      <c r="D35" s="67" t="s">
+        <v>89</v>
       </c>
       <c r="E35" s="50"/>
       <c r="F35" s="50"/>
@@ -3664,13 +3786,13 @@
       <c r="AG35" s="1"/>
     </row>
     <row r="36" spans="1:33" ht="27.75" customHeight="1">
-      <c r="A36" s="104"/>
-      <c r="B36" s="75" t="s">
-        <v>80</v>
-      </c>
-      <c r="C36" s="76"/>
-      <c r="D36" s="96" t="s">
-        <v>119</v>
+      <c r="A36" s="87"/>
+      <c r="B36" s="71" t="s">
+        <v>135</v>
+      </c>
+      <c r="C36" s="72"/>
+      <c r="D36" s="67" t="s">
+        <v>90</v>
       </c>
       <c r="E36" s="50"/>
       <c r="F36" s="50"/>
@@ -3703,13 +3825,13 @@
       <c r="AG36" s="1"/>
     </row>
     <row r="37" spans="1:33" ht="27.75" customHeight="1">
-      <c r="A37" s="104"/>
-      <c r="B37" s="77" t="s">
-        <v>81</v>
-      </c>
-      <c r="C37" s="78"/>
-      <c r="D37" s="99" t="s">
-        <v>121</v>
+      <c r="A37" s="87"/>
+      <c r="B37" s="73" t="s">
+        <v>136</v>
+      </c>
+      <c r="C37" s="74"/>
+      <c r="D37" s="70" t="s">
+        <v>92</v>
       </c>
       <c r="E37" s="50"/>
       <c r="F37" s="50"/>
@@ -3742,13 +3864,13 @@
       <c r="AG37" s="1"/>
     </row>
     <row r="38" spans="1:33" ht="27.75" customHeight="1">
-      <c r="A38" s="105"/>
-      <c r="B38" s="77" t="s">
-        <v>82</v>
-      </c>
-      <c r="C38" s="78"/>
-      <c r="D38" s="99" t="s">
-        <v>120</v>
+      <c r="A38" s="88"/>
+      <c r="B38" s="73" t="s">
+        <v>137</v>
+      </c>
+      <c r="C38" s="74"/>
+      <c r="D38" s="70" t="s">
+        <v>91</v>
       </c>
       <c r="E38" s="50"/>
       <c r="F38" s="50"/>
@@ -3838,16 +3960,19 @@
       <c r="AF40" s="1"/>
       <c r="AG40" s="1"/>
     </row>
-    <row r="41" spans="1:33" ht="15.75" customHeight="1">
+    <row r="41" spans="1:33" ht="12.75">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
+      <c r="F41" s="108"/>
+      <c r="G41" s="109" t="s">
+        <v>102</v>
+      </c>
+      <c r="H41" s="109" t="s">
+        <v>103</v>
+      </c>
+      <c r="I41" s="54"/>
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
@@ -3870,16 +3995,23 @@
       <c r="AF41" s="1"/>
       <c r="AG41" s="1"/>
     </row>
-    <row r="42" spans="1:33" ht="15.75" customHeight="1">
+    <row r="42" spans="1:33" ht="24">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
+      <c r="F42" s="113" t="s">
+        <v>139</v>
+      </c>
+      <c r="G42" s="110" t="s">
+        <v>97</v>
+      </c>
+      <c r="H42" s="110" t="s">
+        <v>104</v>
+      </c>
+      <c r="I42" s="111" t="s">
+        <v>110</v>
+      </c>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
       <c r="L42" s="1"/>
@@ -3910,11 +4042,16 @@
       <c r="B43" s="2"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
+      <c r="F43" s="113" t="s">
+        <v>140</v>
+      </c>
+      <c r="G43" s="110" t="s">
+        <v>98</v>
+      </c>
+      <c r="H43" s="110" t="s">
+        <v>105</v>
+      </c>
+      <c r="I43" s="112"/>
       <c r="L43" s="14"/>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
@@ -3943,14 +4080,16 @@
       <c r="B44" s="2"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="F44" s="114" t="s">
+        <v>141</v>
+      </c>
+      <c r="G44" s="110" t="s">
+        <v>99</v>
+      </c>
+      <c r="H44" s="110" t="s">
+        <v>106</v>
+      </c>
+      <c r="I44" s="112"/>
       <c r="K44" s="1"/>
       <c r="L44" s="2"/>
       <c r="M44" s="1"/>
@@ -3980,13 +4119,17 @@
       <c r="B45" s="2"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="1" t="s">
-        <v>54</v>
+      <c r="F45" s="53" t="s">
+        <v>142</v>
+      </c>
+      <c r="G45" s="110" t="s">
+        <v>100</v>
+      </c>
+      <c r="H45" s="110" t="s">
+        <v>108</v>
+      </c>
+      <c r="I45" s="112" t="s">
+        <v>109</v>
       </c>
       <c r="K45" s="1"/>
       <c r="L45" s="2"/>
@@ -4017,14 +4160,16 @@
       <c r="B46" s="2"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="1" t="s">
-        <v>53</v>
-      </c>
+      <c r="F46" s="114" t="s">
+        <v>143</v>
+      </c>
+      <c r="G46" s="110" t="s">
+        <v>101</v>
+      </c>
+      <c r="H46" s="110" t="s">
+        <v>107</v>
+      </c>
+      <c r="I46" s="112"/>
       <c r="K46" s="1"/>
       <c r="L46" s="2"/>
       <c r="M46" s="1"/>
@@ -4059,9 +4204,6 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
-      <c r="J47" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="K47" s="1"/>
       <c r="L47" s="2"/>
       <c r="M47" s="1"/>
@@ -4096,9 +4238,6 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
-      <c r="J48" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="K48" s="1"/>
       <c r="L48" s="2"/>
       <c r="M48" s="1"/>
@@ -4163,7 +4302,6 @@
       <c r="B50" s="2"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
-      <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
@@ -4198,7 +4336,6 @@
       <c r="B51" s="2"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
-      <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
@@ -4233,9 +4370,10 @@
       <c r="B52" s="2"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
-      <c r="E52" s="2"/>
       <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
+      <c r="G52" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
@@ -4268,9 +4406,10 @@
       <c r="B53" s="2"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
-      <c r="E53" s="2"/>
       <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
+      <c r="G53" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
@@ -4303,9 +4442,10 @@
       <c r="B54" s="2"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
-      <c r="E54" s="2"/>
       <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
+      <c r="G54" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
@@ -4340,7 +4480,9 @@
       <c r="D55" s="1"/>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
+      <c r="G55" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
@@ -4375,7 +4517,9 @@
       <c r="D56" s="1"/>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
+      <c r="G56" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
@@ -11611,6 +11755,20 @@
     <filterColumn colId="9" hiddenButton="1" showButton="0"/>
   </autoFilter>
   <mergeCells count="25">
+    <mergeCell ref="B2:O3"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B21"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:B13"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="B38:C38"/>
@@ -11622,20 +11780,6 @@
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="A9:A26"/>
     <mergeCell ref="A27:A38"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B21"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B2:O3"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="L7:L8"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>